<commit_message>
stuff av did yay
</commit_message>
<xml_diff>
--- a/NYP_Framework_Week01/App/Maps/DM2213_Map_Level_01_Coloured.xlsx
+++ b/NYP_Framework_Week01/App/Maps/DM2213_Map_Level_01_Coloured.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avxl0\OneDrive\Desktop\School work\Year 2\SP3\SP3\NYP_Framework_Week01\App\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DBB6D-9A62-4753-9FAA-16875DAB6ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160FE51A-B5DA-4771-9CE8-DF378FC1FF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DM2213_Map_Level_01 - Copy" sheetId="1" r:id="rId1"/>
@@ -679,91 +679,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -1133,7 +1049,7 @@
   <dimension ref="A1:AH26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI11" sqref="AI11"/>
+      <selection activeCell="AF12" sqref="AF12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1281,94 +1197,94 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AF2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AG2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AH2" s="2">
         <v>23</v>
@@ -1385,94 +1301,94 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AG3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AH3" s="2">
         <v>22</v>
@@ -1926,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1950,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -1974,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AB8">
         <v>0</v>
@@ -2030,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -2054,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -2078,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AB9">
         <v>0</v>
@@ -2134,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -2158,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -2182,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AB10">
         <v>0</v>
@@ -2238,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -2262,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T11">
         <v>0</v>
@@ -2286,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -2330,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2354,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -2378,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -2434,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2458,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -2482,7 +2398,7 @@
         <v>0</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -2538,7 +2454,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2562,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2586,7 +2502,7 @@
         <v>0</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="X14">
         <v>0</v>
@@ -2642,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2666,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -2690,7 +2606,7 @@
         <v>0</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="X15">
         <v>0</v>
@@ -2862,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2886,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -2910,7 +2826,7 @@
         <v>0</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AB17">
         <v>0</v>
@@ -2966,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2990,7 +2906,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -3014,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="AA18">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AB18">
         <v>0</v>
@@ -3070,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -3094,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T19">
         <v>0</v>
@@ -3118,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="AA19">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AB19">
         <v>0</v>
@@ -3174,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -3198,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="T20">
         <v>0</v>
@@ -3222,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="AA20">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AB20">
         <v>0</v>
@@ -3868,45 +3784,31 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B5:L9 N3:S9 U3:AC9 B12:AG25 B10:AC11 AE3:AG11 AD2:AD11">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+  <conditionalFormatting sqref="L9 B5:C24 B25:I25 L10:M12 N9:R10 V21:AG25 T12:U20 D23:I24 D21:O22 J24:U25 D3:I4 M2:AG4 D5:H7 D8:G10 D11:F13 J12:J13 D14:E16 D17:D19 J23:O23 S21:U23 N11:O11 Q11:R11 D20:I20 L20:O20 P11:P14 N12 I14:J16 L8:R8 T8:W11 S12:S16 V12:V15 L5:AG7 X8:Z15 V16:Z20 AB8:AG20 AA12:AA16 L16:O16 L13:N15 K12:K16">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>300</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:L4 M3:M9">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+  <conditionalFormatting sqref="M9 B3:C4">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>300</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
-      <formula>100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T9 B2:AC2 AE2:AG2">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>300</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>